<commit_message>
Changing max pack to upper limit
</commit_message>
<xml_diff>
--- a/src/grPredicted.xlsx
+++ b/src/grPredicted.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshay/Documents/TranslationDynamics/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{442B2A78-4A04-0745-8DD6-DC6BA3244E40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1FD03F5D-003B-5945-8176-48B626BBE37E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21640" yWindow="3800" windowWidth="17980" windowHeight="16440"/>
+    <workbookView xWindow="2800" yWindow="2120" windowWidth="17980" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="grPredicted" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -859,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G13"/>
+  <dimension ref="A2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,52 +1111,6 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>0.29088910600000001</v>
-      </c>
-      <c r="C12">
-        <v>0.376676234</v>
-      </c>
-      <c r="D12">
-        <v>3.9166608999999998E-2</v>
-      </c>
-      <c r="E12">
-        <v>0.70673194900000003</v>
-      </c>
-      <c r="F12">
-        <v>0.73</v>
-      </c>
-      <c r="G12">
-        <v>0.65700000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>0.29492615</v>
-      </c>
-      <c r="C13">
-        <v>0.421485726</v>
-      </c>
-      <c r="D13">
-        <v>3.5770320000000001E-2</v>
-      </c>
-      <c r="E13">
-        <v>0.75218219500000005</v>
-      </c>
-      <c r="F13">
-        <v>0.72</v>
-      </c>
-      <c r="G13">
-        <v>0.64800000000000002</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>